<commit_message>
Manjsi popravki excel fila
</commit_message>
<xml_diff>
--- a/tex/grafi.xlsx
+++ b/tex/grafi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>1 rpi</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Izmerjeni časi: 1 datoteka, različne velikosti datoteke</t>
+  </si>
+  <si>
+    <t>Razlićno število datotek</t>
+  </si>
+  <si>
+    <t>Ne bom uporabil, ker je usseless</t>
+  </si>
+  <si>
+    <t>pretočnost</t>
+  </si>
+  <si>
+    <t>TODO check</t>
   </si>
 </sst>
 </file>
@@ -269,31 +281,69 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56611584"/>
-        <c:axId val="56605696"/>
+        <c:axId val="107107072"/>
+        <c:axId val="107108608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56611584"/>
+        <c:axId val="107107072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Število datotek</a:t>
+                </a:r>
+                <a:endParaRPr lang="sl-SI"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56605696"/>
+        <c:crossAx val="107108608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56605696"/>
+        <c:axId val="107108608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Čas zahtebka (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="sl-SI"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56611584"/>
+        <c:crossAx val="107107072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -306,7 +356,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -491,23 +541,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69649152"/>
-        <c:axId val="69630208"/>
+        <c:axId val="107133952"/>
+        <c:axId val="107135744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69649152"/>
+        <c:axId val="107133952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69630208"/>
+        <c:crossAx val="107135744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69630208"/>
+        <c:axId val="107135744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +565,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69649152"/>
+        <c:crossAx val="107133952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -528,7 +578,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -713,23 +763,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70613632"/>
-        <c:axId val="70612096"/>
+        <c:axId val="107038208"/>
+        <c:axId val="107039744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70613632"/>
+        <c:axId val="107038208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70612096"/>
+        <c:crossAx val="107039744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70612096"/>
+        <c:axId val="107039744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +787,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70613632"/>
+        <c:crossAx val="107038208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -750,7 +800,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -935,23 +985,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="104191104"/>
-        <c:axId val="104189312"/>
+        <c:axId val="107352064"/>
+        <c:axId val="107353600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104191104"/>
+        <c:axId val="107352064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104189312"/>
+        <c:crossAx val="107353600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104189312"/>
+        <c:axId val="107353600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +1009,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104191104"/>
+        <c:crossAx val="107352064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -972,7 +1022,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1157,23 +1207,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69684224"/>
-        <c:axId val="59980800"/>
+        <c:axId val="107387136"/>
+        <c:axId val="107397120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69684224"/>
+        <c:axId val="107387136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59980800"/>
+        <c:crossAx val="107397120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59980800"/>
+        <c:axId val="107397120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1181,7 +1231,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69684224"/>
+        <c:crossAx val="107387136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1194,7 +1244,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1380,25 +1430,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91436160"/>
-        <c:axId val="107944192"/>
+        <c:axId val="107492096"/>
+        <c:axId val="107493632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91436160"/>
+        <c:axId val="107492096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107944192"/>
+        <c:crossAx val="107493632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107944192"/>
+        <c:axId val="107493632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1456,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91436160"/>
+        <c:crossAx val="107492096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1419,7 +1469,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1429,16 +1479,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1897,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1912,6 +1962,9 @@
       </c>
     </row>
     <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -2095,6 +2148,9 @@
       </c>
     </row>
     <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
       <c r="C34">
         <v>1</v>
       </c>
@@ -2318,6 +2374,9 @@
       </c>
     </row>
     <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
       <c r="C56">
         <v>1</v>
       </c>
@@ -2569,6 +2628,9 @@
       </c>
     </row>
     <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
       <c r="C78">
         <v>1</v>
       </c>

</xml_diff>